<commit_message>
school 30 may 2019
</commit_message>
<xml_diff>
--- a/school/timetable.xlsx
+++ b/school/timetable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gits\files\school\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B486073-3945-438E-AADF-6837F573333A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DC06AA-D18D-4D4B-BCDA-30FB208347F8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D7B74CE8-4647-4A0C-A0D6-9F4FBDC4F0B9}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="47">
   <si>
     <t>PERIOD</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>Lunch 12.50 - 13.30</t>
+  </si>
+  <si>
+    <t>#1</t>
   </si>
 </sst>
 </file>
@@ -360,15 +363,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -378,31 +372,29 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="4">
     <dxf>
-      <font>
-        <color rgb="FFF8C7FF"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8C7FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF97009C"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8C7FF"/>
-        </patternFill>
-      </fill>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <border>
@@ -437,6 +429,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF0000FF"/>
+      <color rgb="FF00FF00"/>
+      <color rgb="FFFF00FF"/>
+      <color rgb="FF00FFFF"/>
       <color rgb="FFF8C7FF"/>
       <color rgb="FF97009C"/>
       <color rgb="FFC7CEFF"/>
@@ -459,15 +455,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -537,15 +533,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -615,15 +611,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -693,15 +689,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -771,15 +767,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>191626</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>572626</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -849,15 +845,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>1126</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>191626</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -927,15 +923,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>763126</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1126</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1005,15 +1001,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>572626</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>763126</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1083,15 +1079,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>98534</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1459,447 +1455,462 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8C18104-4931-463F-A89A-A0F4AE622474}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="B2:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="152" zoomScaleNormal="152" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" style="1" customWidth="1"/>
-    <col min="2" max="5" width="14.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" style="1" customWidth="1"/>
-    <col min="7" max="8" width="14.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="1" customWidth="1"/>
-    <col min="10" max="12" width="14.28515625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="10" style="1" customWidth="1"/>
+    <col min="3" max="6" width="14.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" style="1" customWidth="1"/>
+    <col min="8" max="9" width="14.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" style="1" customWidth="1"/>
+    <col min="11" max="13" width="14.28515625" style="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="6">
+      <c r="D2" s="6">
         <v>1</v>
       </c>
-      <c r="D1" s="6">
+      <c r="E2" s="6">
         <v>2</v>
       </c>
-      <c r="E1" s="11">
+      <c r="F2" s="11">
         <v>3</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G2" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="9">
+      <c r="H2" s="9">
         <v>4</v>
       </c>
-      <c r="H1" s="8">
+      <c r="I2" s="8">
         <v>5</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="J2" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="J1" s="9">
+      <c r="K2" s="9">
         <v>6</v>
       </c>
-      <c r="K1" s="6">
+      <c r="L2" s="6">
         <v>7</v>
       </c>
-      <c r="L1" s="6">
+      <c r="M2" s="6">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="C3" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="D3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="E3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="F3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="7" t="s">
+      <c r="G3" s="15"/>
+      <c r="H3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="7" t="s">
+      <c r="J3" s="15"/>
+      <c r="K3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="C4" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="D4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="F4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="14"/>
-      <c r="G3" s="17" t="s">
+      <c r="G4" s="16"/>
+      <c r="H4" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="I4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="14"/>
-      <c r="J3" s="10" t="s">
+      <c r="J4" s="16"/>
+      <c r="K4" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="L4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="M4" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3" t="s">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="17"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="3" t="s">
+      <c r="G5" s="16"/>
+      <c r="H5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="14"/>
-      <c r="J4" s="3" t="s">
+      <c r="J5" s="16"/>
+      <c r="K5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="L5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="C6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="E6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="F6" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="17" t="s">
+      <c r="G6" s="16"/>
+      <c r="H6" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="I6" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I5" s="14"/>
-      <c r="J5" s="17" t="s">
+      <c r="J6" s="16"/>
+      <c r="K6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="L6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="M6" s="14" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3" t="s">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="17"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="3" t="s">
+      <c r="G7" s="16"/>
+      <c r="H7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="3" t="s">
+      <c r="J7" s="16"/>
+      <c r="K7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="L7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="N6" s="2" t="s">
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="16"/>
+      <c r="K8" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="17"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="16"/>
+      <c r="K9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="16"/>
+      <c r="K10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="17"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="16"/>
+      <c r="H11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" s="16"/>
+      <c r="K11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="16"/>
+      <c r="H12" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" s="16"/>
+      <c r="K12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="17"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="16"/>
+      <c r="H13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" s="16"/>
+      <c r="K13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H17" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="N7" s="4" t="s">
+    <row r="18" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H18" s="4" t="s">
         <v>43</v>
       </c>
+      <c r="I18" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" s="14"/>
-      <c r="J8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="N8" s="5" t="s">
+    <row r="19" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H19" s="5" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="14"/>
-      <c r="J9" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="K9" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="L9" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="14"/>
-      <c r="J11" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="L11" s="17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="I1:I12"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="F1:F12"/>
+    <mergeCell ref="J2:J13"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="G2:G13"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:E3 G3:H3 J3:L3 B5:E5 G5:H5 J5:L5 B7:E7 G7:H7 J7:L7 B9:E9 G9:H9 J9:L9 B11:E11 G11:H11 J11:L11">
-    <cfRule type="expression" dxfId="4" priority="3">
-      <formula>OR(B4=B3)</formula>
+  <conditionalFormatting sqref="C4:F4 H4:I4 K4:M4 C6:F6 H6:I6 K6:M6 C8:F8 H8:I8 K8:M8 C10:F10 H10:I10 K10:M10 C12:F12 H12:I12 K12:M12">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>OR(C5=C4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:E4 G4:H4 J4:L4 B6:E6 G6:H6 J6:L6 B8:E8 G8:H8 J8:L8 B10:E10 G10:H10 J10:L10 B12:E12 G12:H12 J12:L12">
-    <cfRule type="expression" dxfId="3" priority="2">
-      <formula>OR(B3=B4)</formula>
+  <conditionalFormatting sqref="C5:F5 H5:I5 K5:M5 C7:F7 H7:I7 K7:M7 C9:F9 H9:I9 K9:M9 C11:F11 H11:I11 K11:M11 C13:F13 H13:I13 K13:M13">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>OR(C4=C5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:L12">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>NOT(A1=B1)</formula>
+  <conditionalFormatting sqref="B2:L13">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>NOT(B2=C2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M13">
+    <cfRule type="expression" dxfId="0" priority="4">
+      <formula>NOT(M2=N1)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>